<commit_message>
Split chem and Pharma in LPGRbIC and URPbIC
</commit_message>
<xml_diff>
--- a/InputData/io-model/URPbIC/Union Representation Perc by ISIC Code.xlsx
+++ b/InputData/io-model/URPbIC/Union Representation Perc by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\io-model\URPbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CBCE12-F9EF-4E7C-90A3-AAF29F30BDDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE1EEED-7765-4B17-A60A-C3BCC453D516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="450" windowWidth="23115" windowHeight="15465" xr2:uid="{111598D9-CA0B-488C-B665-0CB52396764C}"/>
+    <workbookView xWindow="3210" yWindow="585" windowWidth="24090" windowHeight="16650" xr2:uid="{111598D9-CA0B-488C-B665-0CB52396764C}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="161">
   <si>
     <t>Management, professional, and related occupations</t>
   </si>
@@ -314,9 +314,6 @@
     <t>ISIC 19</t>
   </si>
   <si>
-    <t>ISIC 20T21</t>
-  </si>
-  <si>
     <t>ISIC 22</t>
   </si>
   <si>
@@ -431,9 +428,6 @@
     <t>Coke and refined petroleum products</t>
   </si>
   <si>
-    <t>Chemicals and pharmaceutical products</t>
-  </si>
-  <si>
     <t>Rubber and plastic products</t>
   </si>
   <si>
@@ -513,6 +507,18 @@
   </si>
   <si>
     <t>Share Represented by Unions</t>
+  </si>
+  <si>
+    <t>ISIC 21</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>ISIC 20</t>
   </si>
 </sst>
 </file>
@@ -2457,7 +2463,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA20B78F-BFAE-4D2B-A715-7003FB965387}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2471,16 +2477,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>156</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2488,7 +2494,7 @@
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>'BLS Table 3'!A36</f>
@@ -2504,7 +2510,7 @@
         <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2520,7 +2526,7 @@
         <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2536,7 +2542,7 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2552,7 +2558,7 @@
         <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2568,7 +2574,7 @@
         <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2584,7 +2590,7 @@
         <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2600,7 +2606,7 @@
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2616,7 +2622,7 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2629,10 +2635,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C11" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2645,10 +2651,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="C12" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2661,26 +2667,26 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C13" s="15" t="str">
-        <f>'BLS Table 3'!$A$41</f>
-        <v>Durable goods</v>
+        <f>'BLS Table 3'!$A$42</f>
+        <v>Nondurable goods</v>
       </c>
       <c r="D13">
         <f>VLOOKUP($C13,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
-        <v>9.6000000000000002E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C14" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2693,10 +2699,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C15" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2709,10 +2715,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C16" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2725,10 +2731,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C17" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2741,10 +2747,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C18" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2757,10 +2763,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C19" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2773,10 +2779,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C20" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2789,273 +2795,289 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C21" s="15" t="str">
+        <f>'BLS Table 3'!$A$41</f>
+        <v>Durable goods</v>
+      </c>
+      <c r="D21">
+        <f>VLOOKUP($C21,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="15" t="str">
         <f>'BLS Table 3'!A40</f>
         <v>Manufacturing</v>
       </c>
-      <c r="D21">
-        <f>VLOOKUP($C21,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D22">
+        <f>VLOOKUP($C22,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="15" t="str">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="15" t="str">
         <f>'BLS Table 3'!A48</f>
         <v>Utilities</v>
       </c>
-      <c r="D22">
-        <f>VLOOKUP($C22,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D23">
+        <f>VLOOKUP($C23,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="15" t="str">
+      <c r="C24" s="15" t="str">
         <f>'BLS Table 3'!A39</f>
         <v>Construction</v>
       </c>
-      <c r="D23">
-        <f>VLOOKUP($C23,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D24">
+        <f>VLOOKUP($C24,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="15" t="str">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="15" t="str">
         <f>'BLS Table 3'!A43</f>
         <v>Wholesale and retail trade</v>
       </c>
-      <c r="D24">
-        <f>VLOOKUP($C24,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D25">
+        <f>VLOOKUP($C25,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="15" t="str">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="15" t="str">
         <f>'BLS Table 3'!A47</f>
         <v>Transportation and warehousing</v>
       </c>
-      <c r="D25">
-        <f>VLOOKUP($C25,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D26">
+        <f>VLOOKUP($C26,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="15" t="str">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="15" t="str">
         <f>'BLS Table 3'!A67</f>
         <v>Accommodation and food services</v>
       </c>
-      <c r="D26">
-        <f>VLOOKUP($C26,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D27">
+        <f>VLOOKUP($C27,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>2.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="15" t="str">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="15" t="str">
         <f>'BLS Table 3'!A49</f>
         <v>Information(3)</v>
       </c>
-      <c r="D27">
-        <f>VLOOKUP($C27,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D28">
+        <f>VLOOKUP($C28,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.11199999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="15" t="str">
+      <c r="C29" s="15" t="str">
         <f>'BLS Table 3'!A53</f>
         <v>Telecommunications</v>
       </c>
-      <c r="D28">
-        <f>VLOOKUP($C28,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D29">
+        <f>VLOOKUP($C29,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.153</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="15" t="str">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="15" t="str">
         <f>'BLS Table 3'!A60</f>
         <v>Professional and technical services</v>
       </c>
-      <c r="D29">
-        <f>VLOOKUP($C29,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D30">
+        <f>VLOOKUP($C30,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="15" t="str">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="15" t="str">
         <f>'BLS Table 3'!A55</f>
         <v>Finance and insurance</v>
       </c>
-      <c r="D30">
-        <f>VLOOKUP($C30,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D31">
+        <f>VLOOKUP($C31,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="15" t="str">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="15" t="str">
         <f>'BLS Table 3'!A58</f>
         <v>Real estate and rental and leasing</v>
       </c>
-      <c r="D31">
-        <f>VLOOKUP($C31,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D32">
+        <f>VLOOKUP($C32,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="15" t="str">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="15" t="str">
         <f>'BLS Table 3'!A59</f>
         <v>Professional and business services</v>
       </c>
-      <c r="D32">
-        <f>VLOOKUP($C32,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D33">
+        <f>VLOOKUP($C33,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" s="15" t="str">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="15" t="str">
         <f>'BLS Table 3'!A73</f>
         <v>Federal government</v>
       </c>
-      <c r="D33">
-        <f>VLOOKUP($C33,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D34">
+        <f>VLOOKUP($C34,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="15" t="str">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="15" t="str">
         <f>'BLS Table 3'!A14</f>
         <v>Education, training, and library occupations</v>
       </c>
-      <c r="D34">
-        <f>VLOOKUP($C34,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D35">
+        <f>VLOOKUP($C35,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.36599999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B35" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="15" t="str">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="15" t="str">
         <f>'BLS Table 3'!A64</f>
         <v>Health care and social assistance</v>
       </c>
-      <c r="D35">
-        <f>VLOOKUP($C35,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D36">
+        <f>VLOOKUP($C36,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" s="15" t="str">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="15" t="str">
         <f>'BLS Table 3'!A66</f>
         <v>Arts, entertainment, and recreation</v>
       </c>
-      <c r="D36">
-        <f>VLOOKUP($C36,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D37">
+        <f>VLOOKUP($C37,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>7.400000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="15" t="str">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="15" t="str">
         <f>'BLS Table 3'!A70</f>
         <v>Other services(3)</v>
       </c>
-      <c r="D37">
-        <f>VLOOKUP($C37,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D38">
+        <f>VLOOKUP($C38,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
@@ -3069,19 +3091,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="37" width="11.5703125" customWidth="1"/>
+    <col min="2" max="38" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>83</v>
@@ -3111,233 +3133,240 @@
         <v>91</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="AK1" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2">
-        <f>VLOOKUP(B$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(B$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>2.7999999999999997E-2</v>
       </c>
       <c r="C2">
-        <f>VLOOKUP(C$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(C$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
       <c r="D2">
-        <f>VLOOKUP(D$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(D$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
       <c r="E2">
-        <f>VLOOKUP(E$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(E$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
       <c r="F2">
-        <f>VLOOKUP(F$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(F$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="G2">
-        <f>VLOOKUP(G$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(G$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="H2">
-        <f>VLOOKUP(H$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(H$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I2">
-        <f>VLOOKUP(I$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(I$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="J2">
-        <f>VLOOKUP(J$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(J$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="K2">
-        <f>VLOOKUP(K$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(K$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="L2">
-        <f>VLOOKUP(L$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(L$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="M2">
-        <f>VLOOKUP(M$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(M$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="N2">
+        <f>VLOOKUP(N$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="N2">
-        <f>VLOOKUP(N$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="O2">
+        <f>VLOOKUP(O$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="O2">
-        <f>VLOOKUP(O$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="P2">
+        <f>VLOOKUP(P$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="P2">
-        <f>VLOOKUP(P$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="Q2">
+        <f>VLOOKUP(Q$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="Q2">
-        <f>VLOOKUP(Q$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="R2">
+        <f>VLOOKUP(R$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="R2">
-        <f>VLOOKUP(R$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="S2">
+        <f>VLOOKUP(S$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="S2">
-        <f>VLOOKUP(S$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="T2">
+        <f>VLOOKUP(T$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="T2">
-        <f>VLOOKUP(T$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="U2">
+        <f>VLOOKUP(U$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="U2">
-        <f>VLOOKUP(U$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="V2">
+        <f>VLOOKUP(V$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.4E-2</v>
       </c>
-      <c r="V2">
-        <f>VLOOKUP(V$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="W2">
+        <f>VLOOKUP(W$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.24</v>
       </c>
-      <c r="W2">
-        <f>VLOOKUP(W$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="X2">
+        <f>VLOOKUP(X$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.13600000000000001</v>
       </c>
-      <c r="X2">
-        <f>VLOOKUP(X$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="Y2">
+        <f>VLOOKUP(Y$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="Y2">
-        <f>VLOOKUP(Y$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="Z2">
+        <f>VLOOKUP(Z$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.17600000000000002</v>
       </c>
-      <c r="Z2">
-        <f>VLOOKUP(Z$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AA2">
+        <f>VLOOKUP(AA$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AA2">
-        <f>VLOOKUP(AA$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AB2">
+        <f>VLOOKUP(AB$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.11199999999999999</v>
       </c>
-      <c r="AB2">
-        <f>VLOOKUP(AB$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AC2">
+        <f>VLOOKUP(AC$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.153</v>
       </c>
-      <c r="AC2">
-        <f>VLOOKUP(AC$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AD2">
+        <f>VLOOKUP(AD$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>2.2000000000000002E-2</v>
       </c>
-      <c r="AD2">
-        <f>VLOOKUP(AD$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AE2">
+        <f>VLOOKUP(AE$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="AE2">
-        <f>VLOOKUP(AE$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AF2">
+        <f>VLOOKUP(AF$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
-      <c r="AF2">
-        <f>VLOOKUP(AF$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AG2">
+        <f>VLOOKUP(AG$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.03</v>
       </c>
-      <c r="AG2">
-        <f>VLOOKUP(AG$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AH2">
+        <f>VLOOKUP(AH$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="AH2">
-        <f>VLOOKUP(AH$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AI2">
+        <f>VLOOKUP(AI$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.36599999999999999</v>
       </c>
-      <c r="AI2">
-        <f>VLOOKUP(AI$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AJ2">
+        <f>VLOOKUP(AJ$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="AJ2">
-        <f>VLOOKUP(AJ$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AK2">
+        <f>VLOOKUP(AK$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>7.400000000000001E-2</v>
       </c>
-      <c r="AK2">
-        <f>VLOOKUP(AK$1,'ISIC to BLS Map'!$A$1:$D$37,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AL2">
+        <f>VLOOKUP(AL$1,'ISIC to BLS Map'!$A$1:$D$38,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split ISIC codes in 8 more variables (#89)
</commit_message>
<xml_diff>
--- a/InputData/io-model/URPbIC/Union Representation Perc by ISIC Code.xlsx
+++ b/InputData/io-model/URPbIC/Union Representation Perc by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\io-model\URPbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC6CC0-D32D-45CD-8156-ABD0332C3D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF088B62-E7B5-40D0-8FD5-09D79EE24E3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="780" windowWidth="26295" windowHeight="16380" xr2:uid="{111598D9-CA0B-488C-B665-0CB52396764C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{111598D9-CA0B-488C-B665-0CB52396764C}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ISIC to BLS Map" sheetId="4" r:id="rId3"/>
     <sheet name="URPbIC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="171">
   <si>
     <t>Management, professional, and related occupations</t>
   </si>
@@ -314,12 +314,6 @@
     <t>ISIC 22</t>
   </si>
   <si>
-    <t>ISIC 23</t>
-  </si>
-  <si>
-    <t>ISIC 24</t>
-  </si>
-  <si>
     <t>ISIC 25</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>ISIC 31T33</t>
   </si>
   <si>
-    <t>ISIC 35T39</t>
-  </si>
-  <si>
     <t>ISIC 41T43</t>
   </si>
   <si>
@@ -425,12 +416,6 @@
     <t>Rubber and plastic products</t>
   </si>
   <si>
-    <t>Other non-metallic mineral products</t>
-  </si>
-  <si>
-    <t>Basic metals</t>
-  </si>
-  <si>
     <t>Fabricated metal products</t>
   </si>
   <si>
@@ -452,9 +437,6 @@
     <t>Other manufacturing; repair and installation of machinery and equipment</t>
   </si>
   <si>
-    <t>Electricity, gas, water supply, sewerage, waste and remediation services</t>
-  </si>
-  <si>
     <t>Wholesale and retail trade; repair of motor vehicles</t>
   </si>
   <si>
@@ -525,6 +507,48 @@
   </si>
   <si>
     <t>Oil and gas extraction</t>
+  </si>
+  <si>
+    <t>ISIC 239</t>
+  </si>
+  <si>
+    <t>ISIC 231</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>Cement and other nometallic minerals</t>
+  </si>
+  <si>
+    <t>ISIC 241</t>
+  </si>
+  <si>
+    <t>Iron and steel</t>
+  </si>
+  <si>
+    <t>Other metals</t>
+  </si>
+  <si>
+    <t>ISIC 242</t>
+  </si>
+  <si>
+    <t>ISIC 351</t>
+  </si>
+  <si>
+    <t>ISIC 352T353</t>
+  </si>
+  <si>
+    <t>ISIC 36T39</t>
+  </si>
+  <si>
+    <t>Electricity generation and distribution</t>
+  </si>
+  <si>
+    <t>Energy pipelines and gas processing</t>
+  </si>
+  <si>
+    <t>Water and waste</t>
   </si>
 </sst>
 </file>
@@ -569,7 +593,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,13 +612,118 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -603,7 +732,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -640,6 +769,27 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2469,7 +2619,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA20B78F-BFAE-4D2B-A715-7003FB965387}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2483,24 +2633,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>'BLS Table 3'!A36</f>
@@ -2512,11 +2662,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>160</v>
+      <c r="A3" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C3" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2527,12 +2677,12 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>159</v>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C4" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2548,7 +2698,7 @@
         <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C5" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2564,7 +2714,7 @@
         <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C6" s="15" t="str">
         <f>'BLS Table 3'!A38</f>
@@ -2580,7 +2730,7 @@
         <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2596,7 +2746,7 @@
         <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2612,7 +2762,7 @@
         <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2628,7 +2778,7 @@
         <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C10" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2639,12 +2789,12 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2656,11 +2806,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>158</v>
+      <c r="A12" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C12" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2671,12 +2821,12 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>155</v>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C13" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2687,12 +2837,12 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C14" s="15" t="str">
         <f>'BLS Table 3'!$A$42</f>
@@ -2704,11 +2854,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>92</v>
+      <c r="A15" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="C15" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2719,12 +2869,12 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>93</v>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="C16" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2736,11 +2886,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>94</v>
+      <c r="A17" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="C17" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2751,12 +2901,12 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>95</v>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="C18" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2769,10 +2919,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C19" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2785,10 +2935,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C20" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2801,10 +2951,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C21" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2817,10 +2967,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C22" s="15" t="str">
         <f>'BLS Table 3'!$A$41</f>
@@ -2833,273 +2983,337 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C23" s="15" t="str">
+        <f>'BLS Table 3'!$A$41</f>
+        <v>Durable goods</v>
+      </c>
+      <c r="D23">
+        <f>VLOOKUP($C23,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="15" t="str">
+        <f>'BLS Table 3'!$A$41</f>
+        <v>Durable goods</v>
+      </c>
+      <c r="D24">
+        <f>VLOOKUP($C24,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="15" t="str">
         <f>'BLS Table 3'!A40</f>
         <v>Manufacturing</v>
       </c>
-      <c r="D23">
-        <f>VLOOKUP($C23,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D25">
+        <f>VLOOKUP($C25,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="15" t="str">
-        <f>'BLS Table 3'!A48</f>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="15" t="str">
+        <f>'BLS Table 3'!$A$48</f>
         <v>Utilities</v>
       </c>
-      <c r="D24">
-        <f>VLOOKUP($C24,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D26">
+        <f>VLOOKUP($C26,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="15" t="str">
+        <f>'BLS Table 3'!$A$48</f>
+        <v>Utilities</v>
+      </c>
+      <c r="D27">
+        <f>VLOOKUP($C27,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" s="15" t="str">
+        <f>'BLS Table 3'!$A$48</f>
+        <v>Utilities</v>
+      </c>
+      <c r="D28">
+        <f>VLOOKUP($C28,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="15" t="str">
+      <c r="C29" s="15" t="str">
         <f>'BLS Table 3'!A39</f>
         <v>Construction</v>
       </c>
-      <c r="D25">
-        <f>VLOOKUP($C25,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D29">
+        <f>VLOOKUP($C29,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="15" t="str">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="15" t="str">
         <f>'BLS Table 3'!A43</f>
         <v>Wholesale and retail trade</v>
       </c>
-      <c r="D26">
-        <f>VLOOKUP($C26,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D30">
+        <f>VLOOKUP($C30,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="15" t="str">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="15" t="str">
         <f>'BLS Table 3'!A47</f>
         <v>Transportation and warehousing</v>
       </c>
-      <c r="D27">
-        <f>VLOOKUP($C27,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D31">
+        <f>VLOOKUP($C31,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="15" t="str">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="15" t="str">
         <f>'BLS Table 3'!A67</f>
         <v>Accommodation and food services</v>
       </c>
-      <c r="D28">
-        <f>VLOOKUP($C28,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D32">
+        <f>VLOOKUP($C32,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>2.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" s="15" t="str">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="15" t="str">
         <f>'BLS Table 3'!A49</f>
         <v>Information(3)</v>
       </c>
-      <c r="D29">
-        <f>VLOOKUP($C29,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D33">
+        <f>VLOOKUP($C33,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.11199999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="15" t="str">
+      <c r="C34" s="15" t="str">
         <f>'BLS Table 3'!A53</f>
         <v>Telecommunications</v>
       </c>
-      <c r="D30">
-        <f>VLOOKUP($C30,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D34">
+        <f>VLOOKUP($C34,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.153</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="15" t="str">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="15" t="str">
         <f>'BLS Table 3'!A60</f>
         <v>Professional and technical services</v>
       </c>
-      <c r="D31">
-        <f>VLOOKUP($C31,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D35">
+        <f>VLOOKUP($C35,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="15" t="str">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="15" t="str">
         <f>'BLS Table 3'!A55</f>
         <v>Finance and insurance</v>
       </c>
-      <c r="D32">
-        <f>VLOOKUP($C32,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D36">
+        <f>VLOOKUP($C36,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="15" t="str">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="15" t="str">
         <f>'BLS Table 3'!A58</f>
         <v>Real estate and rental and leasing</v>
       </c>
-      <c r="D33">
-        <f>VLOOKUP($C33,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D37">
+        <f>VLOOKUP($C37,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" s="15" t="str">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="15" t="str">
         <f>'BLS Table 3'!A59</f>
         <v>Professional and business services</v>
       </c>
-      <c r="D34">
-        <f>VLOOKUP($C34,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D38">
+        <f>VLOOKUP($C38,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" s="15" t="str">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="15" t="str">
         <f>'BLS Table 3'!A73</f>
         <v>Federal government</v>
       </c>
-      <c r="D35">
-        <f>VLOOKUP($C35,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D39">
+        <f>VLOOKUP($C39,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" s="15" t="str">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="15" t="str">
         <f>'BLS Table 3'!A14</f>
         <v>Education, training, and library occupations</v>
       </c>
-      <c r="D36">
-        <f>VLOOKUP($C36,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D40">
+        <f>VLOOKUP($C40,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>0.36599999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="15" t="str">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="15" t="str">
         <f>'BLS Table 3'!A64</f>
         <v>Health care and social assistance</v>
       </c>
-      <c r="D37">
-        <f>VLOOKUP($C37,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D41">
+        <f>VLOOKUP($C41,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" t="s">
-        <v>150</v>
-      </c>
-      <c r="C38" s="15" t="str">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="15" t="str">
         <f>'BLS Table 3'!A66</f>
         <v>Arts, entertainment, and recreation</v>
       </c>
-      <c r="D38">
-        <f>VLOOKUP($C38,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D42">
+        <f>VLOOKUP($C42,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>7.400000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C39" s="15" t="str">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="15" t="str">
         <f>'BLS Table 3'!A70</f>
         <v>Other services(3)</v>
       </c>
-      <c r="D39">
-        <f>VLOOKUP($C39,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
+      <c r="D43">
+        <f>VLOOKUP($C43,'BLS Table 3'!$A$3:$F$75,COLUMN('BLS Table 3'!$F$2),FALSE)/100</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
@@ -3113,28 +3327,28 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="39" width="11.5703125" customWidth="1"/>
+    <col min="2" max="43" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>159</v>
+      <c r="C1" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>84</v>
@@ -3157,245 +3371,273 @@
       <c r="K1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>155</v>
+      <c r="L1" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="Z1" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AK1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>115</v>
       </c>
-      <c r="AM1" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
       <c r="B2">
-        <f>VLOOKUP(B$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(B$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="C2">
-        <f>VLOOKUP(C$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="C2" s="21">
+        <f>VLOOKUP(C$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
-      <c r="D2">
-        <f>VLOOKUP(D$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="D2" s="22">
+        <f>VLOOKUP(D$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
       <c r="E2">
-        <f>VLOOKUP(E$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(E$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
       <c r="F2">
-        <f>VLOOKUP(F$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(F$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
       <c r="G2">
-        <f>VLOOKUP(G$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(G$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="H2">
-        <f>VLOOKUP(H$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(H$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I2">
-        <f>VLOOKUP(I$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(I$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="J2">
-        <f>VLOOKUP(J$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(J$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="K2">
-        <f>VLOOKUP(K$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(K$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="L2">
-        <f>VLOOKUP(L$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="L2" s="21">
+        <f>VLOOKUP(L$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="M2">
-        <f>VLOOKUP(M$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="M2" s="22">
+        <f>VLOOKUP(M$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="N2">
-        <f>VLOOKUP(N$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(N$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="O2">
-        <f>VLOOKUP(O$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="O2" s="21">
+        <f>VLOOKUP(O$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="P2">
-        <f>VLOOKUP(P$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="P2" s="22">
+        <f>VLOOKUP(P$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="Q2">
-        <f>VLOOKUP(Q$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="Q2" s="21">
+        <f>VLOOKUP(Q$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="R2">
-        <f>VLOOKUP(R$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="R2" s="22">
+        <f>VLOOKUP(R$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="S2">
-        <f>VLOOKUP(S$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(S$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="T2">
-        <f>VLOOKUP(T$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(T$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="U2">
-        <f>VLOOKUP(U$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(U$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="V2">
-        <f>VLOOKUP(V$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(V$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="W2">
-        <f>VLOOKUP(W$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <f>VLOOKUP(W$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="X2">
+        <f>VLOOKUP(X$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="Y2">
+        <f>VLOOKUP(Y$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>9.4E-2</v>
       </c>
-      <c r="X2">
-        <f>VLOOKUP(X$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="Z2" s="21">
+        <f>VLOOKUP(Z$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.24</v>
       </c>
-      <c r="Y2">
-        <f>VLOOKUP(Y$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AA2" s="24">
+        <f>VLOOKUP(AA$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <v>0.24</v>
+      </c>
+      <c r="AB2" s="22">
+        <f>VLOOKUP(AB$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+        <v>0.24</v>
+      </c>
+      <c r="AC2">
+        <f>VLOOKUP(AC$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.13600000000000001</v>
       </c>
-      <c r="Z2">
-        <f>VLOOKUP(Z$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AD2">
+        <f>VLOOKUP(AD$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="AA2">
-        <f>VLOOKUP(AA$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AE2">
+        <f>VLOOKUP(AE$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.17600000000000002</v>
       </c>
-      <c r="AB2">
-        <f>VLOOKUP(AB$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AF2">
+        <f>VLOOKUP(AF$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AC2">
-        <f>VLOOKUP(AC$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AG2">
+        <f>VLOOKUP(AG$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.11199999999999999</v>
       </c>
-      <c r="AD2">
-        <f>VLOOKUP(AD$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AH2">
+        <f>VLOOKUP(AH$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.153</v>
       </c>
-      <c r="AE2">
-        <f>VLOOKUP(AE$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AI2">
+        <f>VLOOKUP(AI$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>2.2000000000000002E-2</v>
       </c>
-      <c r="AF2">
-        <f>VLOOKUP(AF$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AJ2">
+        <f>VLOOKUP(AJ$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="AG2">
-        <f>VLOOKUP(AG$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AK2">
+        <f>VLOOKUP(AK$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>4.7E-2</v>
       </c>
-      <c r="AH2">
-        <f>VLOOKUP(AH$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AL2">
+        <f>VLOOKUP(AL$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.03</v>
       </c>
-      <c r="AI2">
-        <f>VLOOKUP(AI$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AM2">
+        <f>VLOOKUP(AM$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="AJ2">
-        <f>VLOOKUP(AJ$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AN2">
+        <f>VLOOKUP(AN$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>0.36599999999999999</v>
       </c>
-      <c r="AK2">
-        <f>VLOOKUP(AK$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AO2">
+        <f>VLOOKUP(AO$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="AL2">
-        <f>VLOOKUP(AL$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AP2">
+        <f>VLOOKUP(AP$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>7.400000000000001E-2</v>
       </c>
-      <c r="AM2">
-        <f>VLOOKUP(AM$1,'ISIC to BLS Map'!$A$1:$D$39,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
+      <c r="AQ2">
+        <f>VLOOKUP(AQ$1,'ISIC to BLS Map'!$A$1:$D$43,COLUMN('ISIC to BLS Map'!$D$1),FALSE)</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>

</xml_diff>